<commit_message>
update release json + habilitations
</commit_message>
<xml_diff>
--- a/docs/orga/habilitations.xlsx
+++ b/docs/orga/habilitations.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$3:$E$21</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>Nom</t>
   </si>
@@ -201,6 +201,27 @@
   </si>
   <si>
     <t>oussama-smiri</t>
+  </si>
+  <si>
+    <t>BENKECHIKECH</t>
+  </si>
+  <si>
+    <t>Aminechakr</t>
+  </si>
+  <si>
+    <t>MedEIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IssamAxaTech </t>
+  </si>
+  <si>
+    <t>braadil</t>
+  </si>
+  <si>
+    <t>MeriemHamdaoui</t>
+  </si>
+  <si>
+    <t>hrsanaa</t>
   </si>
 </sst>
 </file>
@@ -629,15 +650,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.28515625" bestFit="1" customWidth="1"/>
@@ -677,7 +696,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>50</v>
@@ -723,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -807,7 +826,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -849,7 +868,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -905,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -919,7 +938,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -933,11 +952,11 @@
         <v>5</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E3"/>
+  <autoFilter ref="B3:E21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>